<commit_message>
Revert "update ToddBrown Branch"
</commit_message>
<xml_diff>
--- a/ISRaD_data_files/Kaiser_2007.xlsx
+++ b/ISRaD_data_files/Kaiser_2007.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Agatha/Desktop/Jena/Missing info list/Ready/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{604678E4-0123-0642-AF2E-BC4F5EA9D572}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -23,7 +17,7 @@
     <sheet name="incubation" sheetId="8" r:id="rId8"/>
     <sheet name="controlled vocabulary" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1"/>
+  <calcPr calcId="0" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -531,6 +525,9 @@
     <t>305.77</t>
   </si>
   <si>
+    <t>Gel</t>
+  </si>
+  <si>
     <t>USDA</t>
   </si>
   <si>
@@ -2774,15 +2771,12 @@
   </si>
   <si>
     <t>frc_fraction_modern_sd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gelisol </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2876,14 +2870,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -3165,14 +3151,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3222,7 +3208,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3269,7 +3255,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3307,7 +3293,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3360,14 +3346,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3390,7 +3376,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3413,7 +3399,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3430,7 +3416,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3459,16 +3445,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3578,7 +3562,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3688,7 +3672,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3783,7 +3767,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -3803,16 +3787,16 @@
         <v>164</v>
       </c>
       <c r="N4" t="s">
-        <v>913</v>
+        <v>165</v>
       </c>
       <c r="P4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="U4" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -3827,14 +3811,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3848,106 +3832,106 @@
         <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="I1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K1" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="N1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="O1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="P1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="R1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="S1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="T1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="U1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="V1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="W1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="X1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="Y1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Z1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AA1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="AB1" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="AC1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="AD1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AE1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="AF1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="AG1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="AH1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AI1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AJ1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="AK1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -3958,106 +3942,106 @@
         <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="J2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="M2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="N2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="O2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="P2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="Q2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="R2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="S2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="T2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="U2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="V2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="W2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="X2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="Y2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="Z2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="AA2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="AB2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="AC2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AD2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AE2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AF2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="AG2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="AH2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="AI2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="AJ2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="AK2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4077,25 +4061,25 @@
         <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="M3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="N3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="P3" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="Q3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="R3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="S3" t="s">
         <v>142</v>
@@ -4104,7 +4088,7 @@
         <v>142</v>
       </c>
       <c r="U3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="V3" t="s">
         <v>148</v>
@@ -4113,28 +4097,28 @@
         <v>148</v>
       </c>
       <c r="Z3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AA3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AB3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AC3" t="s">
+        <v>245</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>246</v>
+      </c>
+      <c r="AF3" t="s">
         <v>244</v>
       </c>
-      <c r="AE3" t="s">
-        <v>245</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>243</v>
-      </c>
       <c r="AG3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AH3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4149,19 +4133,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CT9"/>
   <sheetViews>
     <sheetView topLeftCell="AD1" workbookViewId="0">
       <selection activeCell="AZ4" sqref="AZ4:AZ9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:98">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4172,292 +4156,292 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="J1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="K1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="O1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="P1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Q1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="R1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="S1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="T1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="U1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="V1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="W1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="X1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="Y1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="Z1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AA1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AB1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AC1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AD1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AE1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AF1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AG1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="AH1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AI1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AJ1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AK1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AL1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AM1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AN1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AO1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="AP1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="AQ1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="AR1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="AS1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="AT1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AU1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AV1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AW1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AX1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AY1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AZ1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="BA1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="BB1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="BC1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="BD1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="BE1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="BF1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="BG1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="BH1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="BI1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="BJ1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="BK1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="BL1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="BM1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="BN1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="BO1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="BP1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="BQ1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="BR1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="BS1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="BT1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="BU1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="BV1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="BW1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="BX1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="BY1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="BZ1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="CA1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="CB1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CC1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="CD1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="CE1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="CF1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="CG1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="CH1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="CI1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="CJ1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="CK1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="CL1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="CM1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="CN1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="CO1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="CP1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="CQ1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="CR1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="CS1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="CT1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:98">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -4468,292 +4452,292 @@
         <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="I2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="J2" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="K2" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="L2" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="M2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="N2" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="O2" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="P2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="Q2" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="R2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="S2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="T2" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="U2" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="V2" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="W2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="X2" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="Y2" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="Z2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AA2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AB2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AC2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AD2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AE2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AF2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AG2" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AH2" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AI2" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AJ2" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AK2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AL2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AM2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AN2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AO2" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AP2" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AQ2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AR2" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AS2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AT2" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AU2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AV2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AW2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AX2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AY2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AZ2" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="BA2" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="BB2" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="BC2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="BD2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="BE2" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="BF2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="BG2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="BH2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="BI2" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="BJ2" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="BK2" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="BL2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="BM2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="BN2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="BO2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="BP2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="BQ2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="BR2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="BS2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="BT2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="BU2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="BV2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="BW2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="BX2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="BY2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="BZ2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="CA2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="CB2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="CC2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="CD2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="CE2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="CF2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="CG2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="CH2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="CI2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="CJ2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="CK2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="CL2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="CM2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="CN2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="CO2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="CP2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="CQ2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="CR2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="CS2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="CT2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:98">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -4779,13 +4763,13 @@
         <v>142</v>
       </c>
       <c r="O3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="P3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="Q3" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="S3" t="s">
         <v>148</v>
@@ -4803,34 +4787,34 @@
         <v>36</v>
       </c>
       <c r="X3" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AC3" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AD3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="AE3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AF3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AG3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AH3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AI3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AJ3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AK3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AL3" t="s">
         <v>148</v>
@@ -4854,145 +4838,145 @@
         <v>148</v>
       </c>
       <c r="AS3" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AT3" t="s">
         <v>148</v>
       </c>
       <c r="AU3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AV3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AW3" t="s">
+        <v>245</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>246</v>
+      </c>
+      <c r="AZ3" t="s">
         <v>244</v>
       </c>
-      <c r="AY3" t="s">
-        <v>245</v>
-      </c>
-      <c r="AZ3" t="s">
-        <v>243</v>
-      </c>
       <c r="BA3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="BB3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="BE3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="BF3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="BG3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="BH3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="BL3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BM3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BN3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BO3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BQ3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BR3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BS3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BT3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BV3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BW3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BX3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BY3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="BZ3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="CA3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="CB3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="CC3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="CD3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="CE3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CF3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CG3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CH3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CI3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CJ3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CK3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CL3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CM3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CN3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CO3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CP3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CQ3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CR3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CS3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="CT3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:98">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -5003,34 +4987,34 @@
         <v>161</v>
       </c>
       <c r="D4" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="E4" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I4" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="J4" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="K4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="P4" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AO4" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AR4" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="BC4" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:98">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -5041,34 +5025,34 @@
         <v>161</v>
       </c>
       <c r="D5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E5" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I5" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="J5" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="K5" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="P5" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AO5" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AR5" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="BC5" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:98">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -5079,34 +5063,34 @@
         <v>161</v>
       </c>
       <c r="D6" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E6" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I6" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="J6" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="K6" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="P6" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AO6" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="AR6" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="BC6" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
-    <row r="7" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:98">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -5117,34 +5101,34 @@
         <v>161</v>
       </c>
       <c r="D7" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E7" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I7" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="J7" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="K7" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="P7" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AO7" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AR7" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="BC7" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
-    <row r="8" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:98">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -5155,34 +5139,34 @@
         <v>161</v>
       </c>
       <c r="D8" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="E8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I8" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="J8" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="K8" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="P8" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="AO8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AR8" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="BC8" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
-    <row r="9" spans="1:98" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:98">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -5193,31 +5177,31 @@
         <v>161</v>
       </c>
       <c r="D9" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E9" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I9" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="J9" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="K9" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="P9" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="AO9" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AR9" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="BC9" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -5232,14 +5216,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5250,82 +5234,82 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="E1" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F1" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="G1" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="H1" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="I1" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="J1" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="K1" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="L1" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="M1" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="N1" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="O1" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="P1" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="Q1" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="R1" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="S1" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="T1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="U1" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="V1" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="W1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="X1" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="Y1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="Z1" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AA1" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AB1" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5336,79 +5320,79 @@
         <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="H2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="I2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="J2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="K2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="L2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="M2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="N2" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="O2" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="P2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="R2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="S2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="T2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="U2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="V2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="W2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="X2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="Y2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="Z2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="AA2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AB2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5425,34 +5409,34 @@
         <v>151</v>
       </c>
       <c r="H3" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="L3" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="M3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N3" t="s">
         <v>148</v>
       </c>
       <c r="R3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="S3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="V3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="W3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="X3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="Y3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -5467,16 +5451,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:73" ht="42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:73" ht="52">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5487,217 +5471,217 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F1" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="G1" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="H1" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="I1" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="J1" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="K1" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="L1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="M1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="N1" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="O1" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="P1" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="Q1" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="R1" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="S1" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="T1" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="U1" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="V1" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="W1" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="X1" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="Y1" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="Z1" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="AA1" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AB1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="AC1" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="AD1" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="AE1" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="AF1" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="AG1" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="AH1" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="AJ1" s="2" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="AK1" s="3" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="AL1" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="AM1" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="AN1" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="AO1" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="AP1" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="AQ1" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="AR1" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="AS1" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="AT1" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="AU1" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="AV1" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="AW1" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="AX1" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="AY1" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="AZ1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="BA1" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="BB1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="BC1" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="BD1" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="BE1" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="BF1" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="BG1" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="BH1" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="BI1" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="BJ1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="BK1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="BL1" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="BM1" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="BN1" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="BO1" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="BP1" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="BQ1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="BR1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="BS1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="BT1" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="BU1" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
-    <row r="2" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:73">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5708,231 +5692,231 @@
         <v>109</v>
       </c>
       <c r="D2" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="E2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F2" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="G2" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="H2" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="I2" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="J2" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="K2" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="L2" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="M2" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="N2" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="O2" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="P2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="Q2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="R2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="S2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="U2" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="V2" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="W2" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="X2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="Y2" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="Z2" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="AA2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="AB2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="AC2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="AD2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="AE2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="AF2" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="AG2" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="AH2" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="AI2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="AJ2" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="AK2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="AL2" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AM2" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="AN2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AO2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AP2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="AQ2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AR2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AS2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="AT2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AU2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AV2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AW2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AX2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="AY2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AZ2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="BA2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="BB2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="BC2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="BD2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="BE2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="BF2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="BG2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="BH2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="BI2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="BJ2" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="BK2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="BL2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="BM2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="BN2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="BO2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="BP2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="BQ2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="BR2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="BS2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="BT2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="BU2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:73">
       <c r="A3" t="s">
         <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="G3" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="H3" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="I3" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="M3" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="N3" t="s">
         <v>142</v>
@@ -5965,121 +5949,121 @@
         <v>148</v>
       </c>
       <c r="AA3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AB3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AE3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AF3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AG3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AH3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AL3" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="AM3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AN3" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="AO3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AP3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AQ3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AR3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AT3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AU3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AV3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AW3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AY3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="AZ3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="BA3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="BB3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="BD3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="BE3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="BF3" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="BG3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BH3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BI3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BJ3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BK3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BL3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BM3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BN3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BO3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BP3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BQ3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BR3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BS3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BT3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="BU3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -6094,14 +6078,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -6112,88 +6096,88 @@
         <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E1" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="G1" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="H1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="I1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="J1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="K1" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="L1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="M1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="N1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="O1" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="P1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="Q1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="R1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="S1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="T1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="U1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="V1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="W1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="X1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="Y1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="Z1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="AA1" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="AB1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="AC1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="AD1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -6201,82 +6185,82 @@
         <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="E2" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="F2" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="G2" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="H2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="I2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="J2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="K2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="N2" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="O2" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="P2" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="Q2" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="R2" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="T2" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="U2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="V2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="W2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="X2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="Y2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="Z2" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="AA2" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="AB2" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="AC2" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="AD2" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -6290,37 +6274,37 @@
         <v>37</v>
       </c>
       <c r="K3" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="L3" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="M3" t="s">
         <v>144</v>
       </c>
       <c r="P3" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="Q3" t="s">
         <v>148</v>
       </c>
       <c r="T3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="U3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="X3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="Y3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="Z3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AA3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -6335,148 +6319,148 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44">
       <c r="A1" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="B1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="F1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="G1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="H1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="I1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="J1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="K1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="L1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="M1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="N1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="O1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="P1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="Q1" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="R1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="S1" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="T1" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="U1" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="V1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="W1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="X1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="Y1" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="Z1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="AA1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="AB1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="AC1" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="AD1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="AE1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="AF1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="AG1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="AH1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="AI1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="AJ1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="AK1" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="AL1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="AM1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="AN1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="AO1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="AP1" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="AQ1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="AR1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:44">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -6511,828 +6495,828 @@
         <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="M2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="N2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="O2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="P2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="R2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="T2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="U2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="V2" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="W2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="X2" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="Y2" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="Z2" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="AA2" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="AB2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AC2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="AD2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="AE2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="AF2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="AG2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="AH2" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="AI2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="AJ2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="AK2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="AL2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="AM2" t="s">
+        <v>528</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>532</v>
+      </c>
+      <c r="AO2" t="s">
         <v>527</v>
       </c>
-      <c r="AN2" t="s">
-        <v>531</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>526</v>
-      </c>
       <c r="AP2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AQ2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="AR2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:44">
       <c r="G3" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="H3" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="I3" t="s">
+        <v>718</v>
+      </c>
+      <c r="U3" t="s">
         <v>717</v>
       </c>
-      <c r="U3" t="s">
-        <v>716</v>
-      </c>
       <c r="AM3" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="AO3" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="AP3" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:44">
       <c r="A4" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B4" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C4" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D4" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="E4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F4" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="G4" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="H4" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="I4" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="J4" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="K4" t="s">
         <v>162</v>
       </c>
       <c r="L4" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="M4" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="N4" t="s">
+        <v>732</v>
+      </c>
+      <c r="O4" t="s">
+        <v>733</v>
+      </c>
+      <c r="P4" t="s">
+        <v>734</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>735</v>
+      </c>
+      <c r="R4" t="s">
+        <v>723</v>
+      </c>
+      <c r="S4" t="s">
+        <v>723</v>
+      </c>
+      <c r="T4" t="s">
+        <v>736</v>
+      </c>
+      <c r="U4" t="s">
+        <v>737</v>
+      </c>
+      <c r="V4" t="s">
+        <v>738</v>
+      </c>
+      <c r="W4" t="s">
+        <v>739</v>
+      </c>
+      <c r="X4" t="s">
+        <v>723</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>723</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>740</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>741</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>742</v>
+      </c>
+      <c r="AC4" t="s">
         <v>731</v>
       </c>
-      <c r="O4" t="s">
+      <c r="AD4" t="s">
+        <v>743</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>734</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>744</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>745</v>
+      </c>
+      <c r="AH4" t="s">
         <v>732</v>
       </c>
-      <c r="P4" t="s">
-        <v>733</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>734</v>
-      </c>
-      <c r="R4" t="s">
-        <v>722</v>
-      </c>
-      <c r="S4" t="s">
-        <v>722</v>
-      </c>
-      <c r="T4" t="s">
-        <v>735</v>
-      </c>
-      <c r="U4" t="s">
-        <v>736</v>
-      </c>
-      <c r="V4" t="s">
-        <v>737</v>
-      </c>
-      <c r="W4" t="s">
-        <v>738</v>
-      </c>
-      <c r="X4" t="s">
-        <v>722</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>722</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="AI4" t="s">
+        <v>746</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>747</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>748</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>749</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>750</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>751</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>752</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>753</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>723</v>
+      </c>
+      <c r="AR4" t="s">
         <v>739</v>
       </c>
-      <c r="AA4" t="s">
-        <v>740</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>741</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>730</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>742</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>733</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>743</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>744</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>731</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>745</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>746</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>747</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>748</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>749</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>750</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>751</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>752</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>722</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>738</v>
-      </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:44">
       <c r="A5" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B5" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="D5" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="E5" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="F5" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="G5" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="H5" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="I5" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="J5" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="K5" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="L5" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="M5" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="N5" t="s">
+        <v>766</v>
+      </c>
+      <c r="O5" t="s">
+        <v>767</v>
+      </c>
+      <c r="P5" t="s">
+        <v>768</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>769</v>
+      </c>
+      <c r="T5" t="s">
+        <v>770</v>
+      </c>
+      <c r="U5" t="s">
+        <v>771</v>
+      </c>
+      <c r="V5" t="s">
+        <v>772</v>
+      </c>
+      <c r="W5" t="s">
+        <v>773</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>774</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>775</v>
+      </c>
+      <c r="AC5" t="s">
         <v>765</v>
       </c>
-      <c r="O5" t="s">
+      <c r="AD5" t="s">
+        <v>776</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>768</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>777</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>778</v>
+      </c>
+      <c r="AH5" t="s">
         <v>766</v>
       </c>
-      <c r="P5" t="s">
-        <v>767</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>768</v>
-      </c>
-      <c r="T5" t="s">
-        <v>769</v>
-      </c>
-      <c r="U5" t="s">
-        <v>770</v>
-      </c>
-      <c r="V5" t="s">
-        <v>771</v>
-      </c>
-      <c r="W5" t="s">
-        <v>772</v>
-      </c>
-      <c r="AA5" t="s">
+      <c r="AI5" t="s">
+        <v>779</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>780</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>781</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>782</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>783</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>784</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>785</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>786</v>
+      </c>
+      <c r="AR5" t="s">
         <v>773</v>
       </c>
-      <c r="AB5" t="s">
-        <v>774</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>764</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>775</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>767</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>776</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>777</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>765</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>778</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>779</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>780</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>781</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>782</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>783</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>784</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>785</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>772</v>
-      </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:44">
       <c r="A6" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B6" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="D6" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="E6" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="F6" t="s">
+        <v>791</v>
+      </c>
+      <c r="G6" t="s">
+        <v>792</v>
+      </c>
+      <c r="H6" t="s">
+        <v>793</v>
+      </c>
+      <c r="I6" t="s">
+        <v>794</v>
+      </c>
+      <c r="J6" t="s">
+        <v>795</v>
+      </c>
+      <c r="L6" t="s">
+        <v>796</v>
+      </c>
+      <c r="M6" t="s">
+        <v>797</v>
+      </c>
+      <c r="N6" t="s">
+        <v>798</v>
+      </c>
+      <c r="O6" t="s">
+        <v>799</v>
+      </c>
+      <c r="P6" t="s">
+        <v>800</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>524</v>
+      </c>
+      <c r="T6" t="s">
+        <v>801</v>
+      </c>
+      <c r="U6" t="s">
+        <v>802</v>
+      </c>
+      <c r="V6" t="s">
+        <v>803</v>
+      </c>
+      <c r="W6" t="s">
+        <v>804</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>805</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>806</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>797</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>800</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>807</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>808</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>809</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>810</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>790</v>
       </c>
-      <c r="G6" t="s">
-        <v>791</v>
-      </c>
-      <c r="H6" t="s">
-        <v>792</v>
-      </c>
-      <c r="I6" t="s">
-        <v>793</v>
-      </c>
-      <c r="J6" t="s">
-        <v>794</v>
-      </c>
-      <c r="L6" t="s">
-        <v>795</v>
-      </c>
-      <c r="M6" t="s">
-        <v>796</v>
-      </c>
-      <c r="N6" t="s">
-        <v>797</v>
-      </c>
-      <c r="O6" t="s">
-        <v>798</v>
-      </c>
-      <c r="P6" t="s">
-        <v>799</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>523</v>
-      </c>
-      <c r="T6" t="s">
-        <v>800</v>
-      </c>
-      <c r="U6" t="s">
-        <v>801</v>
-      </c>
-      <c r="V6" t="s">
-        <v>802</v>
-      </c>
-      <c r="W6" t="s">
-        <v>803</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>804</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>805</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>796</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>799</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>806</v>
-      </c>
-      <c r="AG6" t="s">
-        <v>807</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>808</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>809</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>789</v>
-      </c>
       <c r="AM6" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="AN6" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="AO6" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="AP6" t="s">
         <v>36</v>
       </c>
       <c r="AR6" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:44">
       <c r="A7" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B7" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="F7" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="G7" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="H7" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="J7" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="L7" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="M7" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="N7" t="s">
+        <v>822</v>
+      </c>
+      <c r="P7" t="s">
+        <v>823</v>
+      </c>
+      <c r="T7" t="s">
+        <v>824</v>
+      </c>
+      <c r="U7" t="s">
+        <v>825</v>
+      </c>
+      <c r="V7" t="s">
+        <v>826</v>
+      </c>
+      <c r="W7" t="s">
+        <v>827</v>
+      </c>
+      <c r="AC7" t="s">
         <v>821</v>
       </c>
-      <c r="P7" t="s">
-        <v>822</v>
-      </c>
-      <c r="T7" t="s">
+      <c r="AE7" t="s">
         <v>823</v>
       </c>
-      <c r="U7" t="s">
-        <v>824</v>
-      </c>
-      <c r="V7" t="s">
-        <v>825</v>
-      </c>
-      <c r="W7" t="s">
-        <v>826</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>820</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>822</v>
-      </c>
       <c r="AF7" t="s">
+        <v>828</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>829</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>830</v>
+      </c>
+      <c r="AM7" t="s">
+        <v>831</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>832</v>
+      </c>
+      <c r="AO7" t="s">
+        <v>833</v>
+      </c>
+      <c r="AP7" t="s">
+        <v>834</v>
+      </c>
+      <c r="AR7" t="s">
         <v>827</v>
       </c>
-      <c r="AG7" t="s">
-        <v>828</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>829</v>
-      </c>
-      <c r="AM7" t="s">
-        <v>830</v>
-      </c>
-      <c r="AN7" t="s">
-        <v>831</v>
-      </c>
-      <c r="AO7" t="s">
-        <v>832</v>
-      </c>
-      <c r="AP7" t="s">
-        <v>833</v>
-      </c>
-      <c r="AR7" t="s">
-        <v>826</v>
-      </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:44">
       <c r="A8" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B8" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="F8" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="G8" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="H8" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="J8" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="L8" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="M8" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="N8" t="s">
+        <v>843</v>
+      </c>
+      <c r="P8" t="s">
+        <v>844</v>
+      </c>
+      <c r="T8" t="s">
+        <v>845</v>
+      </c>
+      <c r="U8" t="s">
+        <v>846</v>
+      </c>
+      <c r="V8" t="s">
+        <v>847</v>
+      </c>
+      <c r="W8" t="s">
+        <v>790</v>
+      </c>
+      <c r="AC8" t="s">
         <v>842</v>
       </c>
-      <c r="P8" t="s">
-        <v>843</v>
-      </c>
-      <c r="T8" t="s">
+      <c r="AE8" t="s">
         <v>844</v>
       </c>
-      <c r="U8" t="s">
-        <v>845</v>
-      </c>
-      <c r="V8" t="s">
-        <v>846</v>
-      </c>
-      <c r="W8" t="s">
-        <v>789</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>841</v>
-      </c>
-      <c r="AE8" t="s">
-        <v>843</v>
-      </c>
       <c r="AG8" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="AM8" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="AN8" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="AO8" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="AP8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="AR8" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:44">
       <c r="A9" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B9" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="F9" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="G9" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="H9" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="J9" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="L9" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="M9" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="P9" t="s">
+        <v>860</v>
+      </c>
+      <c r="T9" t="s">
+        <v>861</v>
+      </c>
+      <c r="U9" t="s">
+        <v>862</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>863</v>
+      </c>
+      <c r="AG9" t="s">
         <v>859</v>
       </c>
-      <c r="T9" t="s">
-        <v>860</v>
-      </c>
-      <c r="U9" t="s">
-        <v>861</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>862</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>858</v>
-      </c>
       <c r="AM9" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="AN9" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="AO9" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="AP9" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:44">
       <c r="A10" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="B10" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="F10" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="G10" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="H10" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="U10" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="AM10" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="AN10" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="AO10" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="AP10" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:44">
       <c r="B11" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="F11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H11" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="U11" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="AM11" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="AN11" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="AO11" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="AP11" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:44">
       <c r="H12" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="U12" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="AM12" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="AN12" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="AO12" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:44">
       <c r="U13" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="AM13" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="AN13" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="AO13" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:44">
       <c r="U14" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="AN14" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="AO14" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:44">
       <c r="U15" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="AN15" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="AO15" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:44">
       <c r="U16" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="AN16" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="AO16" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
-    <row r="17" spans="40:41" x14ac:dyDescent="0.2">
+    <row r="17" spans="40:41">
       <c r="AN17" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="AO17" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
-    <row r="18" spans="40:41" x14ac:dyDescent="0.2">
+    <row r="18" spans="40:41">
       <c r="AN18" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="AO18" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
-    <row r="19" spans="40:41" x14ac:dyDescent="0.2">
+    <row r="19" spans="40:41">
       <c r="AN19" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="AO19" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
-    <row r="20" spans="40:41" x14ac:dyDescent="0.2">
+    <row r="20" spans="40:41">
       <c r="AN20" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="AO20" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
     </row>
-    <row r="21" spans="40:41" x14ac:dyDescent="0.2">
+    <row r="21" spans="40:41">
       <c r="AN21" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
     </row>
   </sheetData>

</xml_diff>